<commit_message>
SG2042REVB: add Temperature sensor interface
Change-Id: I69ff20bf7e4bc88ba8d08859af0293b629f1d25b

Former-commit-id: c900cc24e6203636d84e7856592f633a4a26e755
</commit_message>
<xml_diff>
--- a/SG2042REVB/config.xlsx
+++ b/SG2042REVB/config.xlsx
@@ -2058,7 +2058,7 @@
         <v>ENABLE</v>
       </c>
       <c r="D2" t="str">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="3">
@@ -2072,7 +2072,7 @@
         <v>ENABLE</v>
       </c>
       <c r="D3" t="str">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="4">
@@ -2086,7 +2086,7 @@
         <v>ENABLE</v>
       </c>
       <c r="D4" t="str">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5">
@@ -2114,7 +2114,7 @@
         <v>ENABLE</v>
       </c>
       <c r="D6" t="str">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="7">
@@ -2170,7 +2170,7 @@
         <v>ENABLE</v>
       </c>
       <c r="D10" t="str">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="11">
@@ -2198,7 +2198,7 @@
         <v>ENABLE</v>
       </c>
       <c r="D12" t="str">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="13">
@@ -2212,7 +2212,7 @@
         <v>ENABLE</v>
       </c>
       <c r="D13" t="str">
-        <v>1000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="14">
@@ -2240,7 +2240,7 @@
         <v>ENABLE</v>
       </c>
       <c r="D15" t="str">
-        <v>1000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="16">

</xml_diff>